<commit_message>
Content managemnt services info updated by deepthi
</commit_message>
<xml_diff>
--- a/FFG Services.xlsx
+++ b/FFG Services.xlsx
@@ -9,11 +9,16 @@
   </sheets>
   <definedNames/>
   <calcPr/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mgY1JW6gejTdJloroXrZ9fjRFK5uQ=="/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="74">
   <si>
     <t>LoginRequest</t>
   </si>
@@ -201,6 +206,18 @@
     <t>UserProfile Details</t>
   </si>
   <si>
+    <t>GetCentersRequest</t>
+  </si>
+  <si>
+    <t>No Input</t>
+  </si>
+  <si>
+    <t>GetCentersResponse</t>
+  </si>
+  <si>
+    <t>list of All cneters</t>
+  </si>
+  <si>
     <t>Profile Details</t>
   </si>
   <si>
@@ -214,19 +231,29 @@
   </si>
   <si>
     <t>Content Management</t>
+  </si>
+  <si>
+    <t>content Type</t>
+  </si>
+  <si>
+    <t>contentViews</t>
+  </si>
+  <si>
+    <t>AssessmentURL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
@@ -235,15 +262,21 @@
       <color rgb="FF974806"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <sz val="11.0"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
     <font/>
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -260,7 +293,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="20">
     <border/>
     <border>
       <left style="medium">
@@ -378,11 +411,54 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -390,32 +466,44 @@
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
     <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="2" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="10" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="14" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="15" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="14" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="16" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="10" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="17" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="18" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="19" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -642,7 +730,7 @@
   <cols>
     <col customWidth="1" min="1" max="2" width="7.63"/>
     <col customWidth="1" min="3" max="3" width="13.5"/>
-    <col customWidth="1" min="4" max="26" width="7.63"/>
+    <col customWidth="1" min="4" max="6" width="7.63"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -1959,7 +2047,7 @@
     <col customWidth="1" min="2" max="2" width="18.0"/>
     <col customWidth="1" min="3" max="3" width="8.38"/>
     <col customWidth="1" min="4" max="4" width="18.25"/>
-    <col customWidth="1" min="5" max="26" width="7.63"/>
+    <col customWidth="1" min="5" max="6" width="7.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1989,32 +2077,32 @@
     <row r="3">
       <c r="A3" s="9"/>
       <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="11" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="9"/>
       <c r="B4" s="10"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12" t="s">
+      <c r="C4" s="1"/>
+      <c r="D4" s="11" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="9"/>
       <c r="B5" s="10"/>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="12"/>
+      <c r="D5" s="11"/>
     </row>
     <row r="6">
-      <c r="A6" s="13"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="16" t="s">
+      <c r="A6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="15" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2025,32 +2113,32 @@
       <c r="B7" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="18"/>
+      <c r="D7" s="17"/>
     </row>
     <row r="8">
       <c r="A8" s="9"/>
       <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="12" t="s">
+      <c r="C8" s="1"/>
+      <c r="D8" s="11" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="9"/>
       <c r="B9" s="10"/>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="12"/>
+      <c r="D9" s="11"/>
     </row>
     <row r="10">
-      <c r="A10" s="13"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16" t="s">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="15" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2061,475 +2149,517 @@
       <c r="B11" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="18"/>
+      <c r="D11" s="17"/>
     </row>
     <row r="12">
       <c r="A12" s="9"/>
       <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="19" t="s">
+      <c r="C12" s="1"/>
+      <c r="D12" s="18" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="9"/>
       <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="19" t="s">
+      <c r="C13" s="1"/>
+      <c r="D13" s="18" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="9"/>
       <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="19" t="s">
+      <c r="C14" s="1"/>
+      <c r="D14" s="18" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="9"/>
       <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="19" t="s">
+      <c r="C15" s="1"/>
+      <c r="D15" s="18" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="9"/>
       <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="12" t="s">
+      <c r="C16" s="1"/>
+      <c r="D16" s="11" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="9"/>
       <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="19" t="s">
+      <c r="C17" s="1"/>
+      <c r="D17" s="18" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="9"/>
       <c r="B18" s="10"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="12" t="s">
+      <c r="C18" s="1"/>
+      <c r="D18" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="9"/>
       <c r="B19" s="10"/>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="12"/>
+      <c r="D19" s="11"/>
     </row>
     <row r="20">
-      <c r="A20" s="13"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="15"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="19"/>
       <c r="D20" s="20" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="5">
-        <v>4.0</v>
-      </c>
-      <c r="B21" s="6" t="s">
+      <c r="A21" s="9"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="18"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
+      <c r="D21" s="22"/>
+    </row>
+    <row r="22">
       <c r="A22" s="9"/>
       <c r="B22" s="10"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
+      <c r="C22" s="23"/>
+      <c r="D22" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23">
       <c r="A23" s="9"/>
       <c r="B23" s="10"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="12"/>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="9"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" s="12"/>
+      <c r="C23" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="26"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="12"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="24" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="9"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="12" t="s">
-        <v>9</v>
-      </c>
+      <c r="A25" s="5">
+        <v>4.0</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="17"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="9"/>
       <c r="B26" s="10"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="12" t="s">
+      <c r="C26" s="1"/>
+      <c r="D26" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="9"/>
       <c r="B27" s="10"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="12" t="s">
-        <v>11</v>
-      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="11"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="9"/>
       <c r="B28" s="10"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="12" t="s">
-        <v>12</v>
-      </c>
+      <c r="C28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="11"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="9"/>
       <c r="B29" s="10"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="12" t="s">
-        <v>13</v>
+      <c r="C29" s="1"/>
+      <c r="D29" s="11" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="9"/>
       <c r="B30" s="10"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="12" t="s">
-        <v>14</v>
+      <c r="C30" s="1"/>
+      <c r="D30" s="11" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="9"/>
       <c r="B31" s="10"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="12" t="s">
-        <v>18</v>
+      <c r="C31" s="1"/>
+      <c r="D31" s="11" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="13"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="16" t="s">
-        <v>19</v>
+      <c r="A32" s="9"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="5">
-        <v>5.0</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C33" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D33" s="18"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="11" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="9"/>
       <c r="B34" s="10"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="12" t="s">
-        <v>26</v>
+      <c r="C34" s="1"/>
+      <c r="D34" s="11" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="9"/>
       <c r="B35" s="10"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="12" t="s">
-        <v>27</v>
+      <c r="C35" s="1"/>
+      <c r="D35" s="11" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="9"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="12" t="s">
-        <v>28</v>
+      <c r="A36" s="12"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="15" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="9"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="12" t="s">
-        <v>29</v>
-      </c>
+      <c r="A37" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="17"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="9"/>
       <c r="B38" s="10"/>
-      <c r="C38" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D38" s="12"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="11" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="13"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="16" t="s">
-        <v>7</v>
+      <c r="A39" s="9"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="11" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="5">
-        <v>6.0</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C40" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D40" s="18"/>
+      <c r="A40" s="9"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="11" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="9"/>
       <c r="B41" s="10"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="12" t="s">
-        <v>32</v>
+      <c r="C41" s="1"/>
+      <c r="D41" s="11" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="9"/>
       <c r="B42" s="10"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="12" t="s">
-        <v>21</v>
-      </c>
+      <c r="C42" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" s="11"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="9"/>
-      <c r="B43" s="10"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="12" t="s">
-        <v>33</v>
+      <c r="A43" s="12"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="9"/>
-      <c r="B44" s="10"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="A44" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D44" s="17"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="9"/>
       <c r="B45" s="10"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="12" t="s">
-        <v>35</v>
+      <c r="C45" s="1"/>
+      <c r="D45" s="11" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="9"/>
       <c r="B46" s="10"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="12" t="s">
-        <v>36</v>
+      <c r="C46" s="1"/>
+      <c r="D46" s="11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="9"/>
       <c r="B47" s="10"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="12" t="s">
-        <v>37</v>
+      <c r="C47" s="1"/>
+      <c r="D47" s="11" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="9"/>
       <c r="B48" s="10"/>
-      <c r="C48" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D48" s="12"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="11" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="13"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="15"/>
-      <c r="D49" s="16" t="s">
-        <v>7</v>
+      <c r="A49" s="9"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="11" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="5">
-        <v>7.0</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C50" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="D50" s="18"/>
+      <c r="A50" s="9"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="11" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="9"/>
       <c r="B51" s="10"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="12" t="s">
-        <v>32</v>
+      <c r="C51" s="1"/>
+      <c r="D51" s="11" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="9"/>
       <c r="B52" s="10"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="12" t="s">
-        <v>21</v>
-      </c>
+      <c r="C52" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D52" s="11"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="9"/>
-      <c r="B53" s="10"/>
-      <c r="C53" s="11"/>
-      <c r="D53" s="12" t="s">
-        <v>33</v>
+      <c r="A53" s="12"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="9"/>
-      <c r="B54" s="10"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="12" t="s">
-        <v>34</v>
-      </c>
+      <c r="A54" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C54" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D54" s="17"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="9"/>
       <c r="B55" s="10"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="12" t="s">
-        <v>35</v>
+      <c r="C55" s="1"/>
+      <c r="D55" s="11" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="9"/>
       <c r="B56" s="10"/>
-      <c r="C56" s="11"/>
-      <c r="D56" s="12" t="s">
-        <v>36</v>
+      <c r="C56" s="1"/>
+      <c r="D56" s="11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="9"/>
       <c r="B57" s="10"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="12" t="s">
-        <v>37</v>
+      <c r="C57" s="1"/>
+      <c r="D57" s="11" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="9"/>
       <c r="B58" s="10"/>
-      <c r="C58" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D58" s="12"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="11" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="13"/>
-      <c r="B59" s="14"/>
-      <c r="C59" s="15"/>
-      <c r="D59" s="16" t="s">
-        <v>7</v>
+      <c r="A59" s="9"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="11" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="5">
-        <v>8.0</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C60" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D60" s="18"/>
+      <c r="A60" s="9"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="11" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="9"/>
       <c r="B61" s="10"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="12" t="s">
-        <v>42</v>
+      <c r="C61" s="1"/>
+      <c r="D61" s="11" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="9"/>
       <c r="B62" s="10"/>
-      <c r="C62" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D62" s="12"/>
+      <c r="C62" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D62" s="11"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="9"/>
-      <c r="B63" s="10"/>
-      <c r="C63" s="11"/>
-      <c r="D63" s="12" t="s">
-        <v>44</v>
+      <c r="A63" s="12"/>
+      <c r="B63" s="13"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="9"/>
-      <c r="B64" s="10"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="12" t="s">
-        <v>45</v>
-      </c>
+      <c r="A64" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C64" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D64" s="17"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="9"/>
       <c r="B65" s="10"/>
-      <c r="C65" s="11"/>
-      <c r="D65" s="12" t="s">
+      <c r="C65" s="1"/>
+      <c r="D65" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="66" ht="15.75" customHeight="1">
+      <c r="A66" s="9"/>
+      <c r="B66" s="10"/>
+      <c r="C66" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D66" s="11"/>
+    </row>
+    <row r="67" ht="15.75" customHeight="1">
+      <c r="A67" s="9"/>
+      <c r="B67" s="10"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="68" ht="15.75" customHeight="1">
+      <c r="A68" s="9"/>
+      <c r="B68" s="10"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="69" ht="15.75" customHeight="1">
+      <c r="A69" s="9"/>
+      <c r="B69" s="10"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="70" ht="15.75" customHeight="1">
+      <c r="A70" s="9"/>
+      <c r="B70" s="10"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="27" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="13"/>
-      <c r="B66" s="14"/>
-      <c r="C66" s="15"/>
-      <c r="D66" s="16" t="s">
+    <row r="71" ht="15.75" customHeight="1">
+      <c r="A71" s="9"/>
+      <c r="B71" s="10"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="72" ht="15.75" customHeight="1">
+      <c r="A72" s="12"/>
+      <c r="B72" s="13"/>
+      <c r="C72" s="14"/>
+      <c r="D72" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="67" ht="15.75" customHeight="1"/>
-    <row r="68" ht="15.75" customHeight="1"/>
-    <row r="69" ht="15.75" customHeight="1"/>
-    <row r="70" ht="15.75" customHeight="1"/>
-    <row r="71" ht="15.75" customHeight="1"/>
-    <row r="72" ht="15.75" customHeight="1"/>
     <row r="73" ht="15.75" customHeight="1"/>
     <row r="74" ht="15.75" customHeight="1"/>
     <row r="75" ht="15.75" customHeight="1"/>
@@ -3459,6 +3589,9 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
     <row r="1001" ht="15.75" customHeight="1"/>
+    <row r="1002" ht="15.75" customHeight="1"/>
+    <row r="1003" ht="15.75" customHeight="1"/>
+    <row r="1004" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="17">
     <mergeCell ref="A2:A6"/>
@@ -3466,18 +3599,18 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A7:A10"/>
     <mergeCell ref="B7:B10"/>
-    <mergeCell ref="A11:A20"/>
-    <mergeCell ref="B11:B20"/>
-    <mergeCell ref="A50:A59"/>
-    <mergeCell ref="A60:A66"/>
-    <mergeCell ref="A21:A32"/>
-    <mergeCell ref="B21:B32"/>
-    <mergeCell ref="A33:A39"/>
-    <mergeCell ref="B33:B39"/>
-    <mergeCell ref="A40:A49"/>
-    <mergeCell ref="B40:B49"/>
-    <mergeCell ref="B50:B59"/>
-    <mergeCell ref="B60:B66"/>
+    <mergeCell ref="A11:A24"/>
+    <mergeCell ref="B11:B24"/>
+    <mergeCell ref="A54:A63"/>
+    <mergeCell ref="A64:A72"/>
+    <mergeCell ref="A25:A36"/>
+    <mergeCell ref="B25:B36"/>
+    <mergeCell ref="A37:A43"/>
+    <mergeCell ref="B37:B43"/>
+    <mergeCell ref="A44:A53"/>
+    <mergeCell ref="B44:B53"/>
+    <mergeCell ref="B54:B63"/>
+    <mergeCell ref="B64:B72"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -3496,7 +3629,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="7.63"/>
+    <col customWidth="1" min="1" max="6" width="7.63"/>
   </cols>
   <sheetData>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>